<commit_message>
updated the latency figures
</commit_message>
<xml_diff>
--- a/Documentation/latency.xlsx
+++ b/Documentation/latency.xlsx
@@ -11,12 +11,71 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcCompleted="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Collins, Diarmuid</author>
+  </authors>
+  <commentList>
+    <comment ref="G34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Collins, Diarmuid:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is what Cassidian saw in their test system. The PCM bandwidth is exceeded and as a result the software playback cannot minimse the latency, possibly due to loss of video data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Collins, Diarmuid:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is a snapshot of ~20 seconds of video analysing the MPEG TS PIDs
+Here you can see the percentage breakdown of the different MPEG packets and get an idea of the overhead. The null packets would be a function of the spare bandwidth over the available PCM bandwidth</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
   <si>
     <t>Video</t>
   </si>
@@ -73,16 +132,81 @@
   </si>
   <si>
     <t>E2E Latency over PCM (ms)</t>
+  </si>
+  <si>
+    <t>Bits per RTP</t>
+  </si>
+  <si>
+    <t>packets/sec</t>
+  </si>
+  <si>
+    <t>buffer 10 seconds</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>PCM setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video words </t>
+  </si>
+  <si>
+    <t>Frame Rate</t>
+  </si>
+  <si>
+    <t>PCM b/w per video (kbps)</t>
+  </si>
+  <si>
+    <t>PAT</t>
+  </si>
+  <si>
+    <t>PMT</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Stereo @ 512k</t>
+  </si>
+  <si>
+    <t>No Audio @512</t>
+  </si>
+  <si>
+    <t>Typical MPEG TS PID @ 781 PCM b/w</t>
+  </si>
+  <si>
+    <t>Stereo @ 750k</t>
+  </si>
+  <si>
+    <t>No Audio @750k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,16 +219,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -112,17 +255,165 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -420,158 +711,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>15</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G2">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5">
+        <f>16*D2*G2*I2/1024</f>
+        <v>968.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
         <v>0.51200000000000001</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="G6">
         <f>860-620</f>
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>0.75</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>0.75</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>0.9</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -582,142 +845,883 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="E7">
         <v>25</v>
       </c>
       <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0.75</v>
+      </c>
+      <c r="E8">
+        <v>12.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.75</v>
+      </c>
+      <c r="E9">
+        <v>12.5</v>
+      </c>
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G7">
+      <c r="G9">
+        <f>730-490</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+      <c r="E10">
+        <v>12.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0.75</v>
+      </c>
+      <c r="E11">
+        <v>8.33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+      <c r="E12">
+        <v>8.33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <f>610-170</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0.75</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <f>780-380</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0.75</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14">
+        <f>740-380</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>0.75</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>0.75</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0.75</v>
+      </c>
+      <c r="E17">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>0.75</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>0.9</v>
+      </c>
+      <c r="E19">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>0.9</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20">
         <f>1000-720</f>
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.9</v>
+      </c>
+      <c r="E21">
+        <v>12.5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <f>570-250</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.9</v>
+      </c>
+      <c r="E22">
+        <v>12.5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <f>490-170</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="E23">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F23" t="s">
         <v>9</v>
       </c>
-      <c r="G8">
+      <c r="G23">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
         <v>15</v>
       </c>
-      <c r="D9">
+      <c r="D24">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="E24">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F24" t="s">
         <v>8</v>
       </c>
-      <c r="G9">
+      <c r="G24">
         <f>950-710</f>
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
         <v>5</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D28" t="s">
         <v>11</v>
       </c>
-      <c r="E17">
+      <c r="E28">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F28" t="s">
         <v>9</v>
       </c>
-      <c r="G17">
+      <c r="G28">
         <f>630-390</f>
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D29" s="1">
         <f>94*16*5*200/(1024*1024)</f>
         <v>1.434326171875</v>
       </c>
-      <c r="E18">
+      <c r="E29">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F29" t="s">
         <v>12</v>
       </c>
-      <c r="G18">
+      <c r="G29">
         <f>990-750</f>
         <v>240</v>
       </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32">
+        <v>200</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="5">
+        <f>16*D32*G32*I32/1024</f>
+        <v>781.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.9</v>
+      </c>
+      <c r="E34">
+        <v>12.5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="11">
+        <f>1560-0</f>
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0.9</v>
+      </c>
+      <c r="E35">
+        <v>12.5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="11">
+        <f>2080-440</f>
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0.75</v>
+      </c>
+      <c r="E36">
+        <v>12.5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <f>730-410</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.75</v>
+      </c>
+      <c r="E37">
+        <v>12.5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <f>730-410</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="E38">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38">
+        <f>810-450</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="E39">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <f>530-250</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="9">
+        <v>16234</v>
+      </c>
+      <c r="C45" s="13">
+        <f>B45/SUM(B$45:B$49)</f>
+        <v>0.66432049760608913</v>
+      </c>
+      <c r="D45" s="14">
+        <v>16251</v>
+      </c>
+      <c r="E45" s="15">
+        <f>D45/SUM(D$45:D$49)</f>
+        <v>0.66501616401358599</v>
+      </c>
+      <c r="F45" s="9">
+        <v>12885</v>
+      </c>
+      <c r="G45" s="13">
+        <f>F45/SUM(F$45:F$49)</f>
+        <v>0.81736868815021568</v>
+      </c>
+      <c r="H45" s="14">
+        <v>14687</v>
+      </c>
+      <c r="I45" s="15">
+        <f>H45/SUM(H$45:H$49)</f>
+        <v>0.93167977670641966</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="9">
+        <v>4946</v>
+      </c>
+      <c r="C46" s="13">
+        <f t="shared" ref="C46:C49" si="0">B46/SUM(B$45:B$49)</f>
+        <v>0.20239800302819494</v>
+      </c>
+      <c r="D46" s="14">
+        <v>0</v>
+      </c>
+      <c r="E46" s="15">
+        <f>D46/SUM(D$45:D$49)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="9">
+        <v>2098</v>
+      </c>
+      <c r="G46" s="13">
+        <f t="shared" ref="G46:G49" si="1">F46/SUM(F$45:F$49)</f>
+        <v>0.13308804871859933</v>
+      </c>
+      <c r="H46" s="14">
+        <v>0</v>
+      </c>
+      <c r="I46" s="15">
+        <f>H46/SUM(H$45:H$49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="9">
+        <v>582</v>
+      </c>
+      <c r="C47" s="13">
+        <f t="shared" si="0"/>
+        <v>2.3816344068420838E-2</v>
+      </c>
+      <c r="D47" s="14">
+        <v>582</v>
+      </c>
+      <c r="E47" s="15">
+        <f>D47/SUM(D$45:D$49)</f>
+        <v>2.3816344068420838E-2</v>
+      </c>
+      <c r="F47" s="9">
+        <v>288</v>
+      </c>
+      <c r="G47" s="13">
+        <f t="shared" si="1"/>
+        <v>1.8269474752600864E-2</v>
+      </c>
+      <c r="H47" s="14">
+        <v>288</v>
+      </c>
+      <c r="I47" s="15">
+        <f>H47/SUM(H$45:H$49)</f>
+        <v>1.8269474752600864E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="9">
+        <v>582</v>
+      </c>
+      <c r="C48" s="13">
+        <f t="shared" si="0"/>
+        <v>2.3816344068420838E-2</v>
+      </c>
+      <c r="D48" s="14">
+        <v>582</v>
+      </c>
+      <c r="E48" s="15">
+        <f>D48/SUM(D$45:D$49)</f>
+        <v>2.3816344068420838E-2</v>
+      </c>
+      <c r="F48" s="9">
+        <v>288</v>
+      </c>
+      <c r="G48" s="13">
+        <f t="shared" si="1"/>
+        <v>1.8269474752600864E-2</v>
+      </c>
+      <c r="H48" s="14">
+        <v>288</v>
+      </c>
+      <c r="I48" s="15">
+        <f>H48/SUM(H$45:H$49)</f>
+        <v>1.8269474752600864E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="10">
+        <v>2093</v>
+      </c>
+      <c r="C49" s="16">
+        <f t="shared" si="0"/>
+        <v>8.5648811228874244E-2</v>
+      </c>
+      <c r="D49" s="17">
+        <v>7022</v>
+      </c>
+      <c r="E49" s="18">
+        <f>D49/SUM(D$45:D$49)</f>
+        <v>0.28735114784957239</v>
+      </c>
+      <c r="F49" s="10">
+        <v>205</v>
+      </c>
+      <c r="G49" s="16">
+        <f t="shared" si="1"/>
+        <v>1.3004313625983253E-2</v>
+      </c>
+      <c r="H49" s="17">
+        <v>501</v>
+      </c>
+      <c r="I49" s="18">
+        <f>H49/SUM(H$45:H$49)</f>
+        <v>3.1781273788378583E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:G7">
     <sortCondition ref="D2:D7"/>
   </sortState>
+  <mergeCells count="4">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F5:H10"/>
+  <dimension ref="F4:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>561</v>
+      </c>
+      <c r="O4" s="3">
+        <f>N4/$N$9</f>
+        <v>1.52044881697699E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>5887</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" ref="O5:O9" si="0">N5/$N$9</f>
+        <v>0.15955226712198825</v>
+      </c>
+    </row>
+    <row r="6" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>14</v>
       </c>
@@ -725,10 +1729,20 @@
         <v>120</v>
       </c>
       <c r="H6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>62</v>
+      </c>
+      <c r="N6">
+        <v>29336</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.79507819063880536</v>
+      </c>
+    </row>
+    <row r="7" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>15</v>
       </c>
@@ -736,10 +1750,20 @@
         <v>5</v>
       </c>
       <c r="H7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>553</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4987668374122557E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>16</v>
       </c>
@@ -749,8 +1773,28 @@
       <c r="H8">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>200</v>
+      </c>
+      <c r="N8">
+        <v>560</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5177385695313982E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <f>SUM(N4:N8)</f>
+        <v>36897</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>17</v>
       </c>
@@ -760,7 +1804,59 @@
       </c>
       <c r="H10">
         <f>H6*16*H7*H8/(1024)</f>
-        <v>2500</v>
+        <v>781.25</v>
+      </c>
+      <c r="I10">
+        <f>I6*16*I7*I8/(1024)</f>
+        <v>968.75</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <f>10*1024*1024</f>
+        <v>10485760</v>
+      </c>
+      <c r="H15">
+        <f>0.5*1024*1024</f>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16">
+        <f>1500*8-1280-32</f>
+        <v>10688</v>
+      </c>
+      <c r="H16">
+        <f>1500*8-1280-32</f>
+        <v>10688</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <f>G15/G16</f>
+        <v>981.07784431137725</v>
+      </c>
+      <c r="H17">
+        <f>H15/H16</f>
+        <v>49.053892215568865</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19">
+        <f>G17*10</f>
+        <v>9810.7784431137734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up the logging output so that we can select the verbosity level from the command line
</commit_message>
<xml_diff>
--- a/Documentation/latency.xlsx
+++ b/Documentation/latency.xlsx
@@ -45,7 +45,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0">
+    <comment ref="A47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Collins, Diarmuid:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is a snapshot of ~20 seconds of video analysing the MPEG TS PIDs
+Here you can see the percentage breakdown of the different MPEG packets and get an idea of the overhead. The null packets would be a function of the spare bandwidth over the available PCM bandwidth</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="48">
   <si>
     <t>Video</t>
   </si>
@@ -183,6 +208,42 @@
   </si>
   <si>
     <t>No Audio @750k</t>
+  </si>
+  <si>
+    <t>visible artifacts</t>
+  </si>
+  <si>
+    <t>Typical MPEG TS PID @ 968k PCM b/w</t>
+  </si>
+  <si>
+    <t>Stereo @ 900k</t>
+  </si>
+  <si>
+    <t>No Audio @900k</t>
+  </si>
+  <si>
+    <t>PCM Frame Rate</t>
+  </si>
+  <si>
+    <t>How test was performed</t>
+  </si>
+  <si>
+    <t>Used GTSDecom to bridge between PCM and UDP</t>
+  </si>
+  <si>
+    <t>Played back video with mplayer on remote PC client</t>
+  </si>
+  <si>
+    <t>Used mplayer -benchmark -nosound as command line</t>
+  </si>
+  <si>
+    <t>Pointed video camera at screen with timestamp visible</t>
+  </si>
+  <si>
+    <t>Paused the playback and subtracted the actual timestamp and the timestamp via the camera</t>
+  </si>
+  <si>
+    <t>Difference was measured latency</t>
   </si>
 </sst>
 </file>
@@ -377,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -387,18 +448,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
@@ -410,6 +462,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I50"/>
+  <dimension ref="A2:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,37 +789,37 @@
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="19">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="19">
         <v>200</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -764,7 +828,7 @@
         <v>968.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -787,7 +851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -810,7 +874,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -833,8 +897,11 @@
         <f>860-620</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -856,8 +923,11 @@
       <c r="G7">
         <v>240</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -879,8 +949,11 @@
       <c r="G8">
         <v>240</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -903,8 +976,11 @@
         <f>730-490</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -926,8 +1002,11 @@
       <c r="G10">
         <v>240</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -949,8 +1028,11 @@
       <c r="G11">
         <v>360</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -973,8 +1055,11 @@
         <f>610-170</f>
         <v>440</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -998,7 +1083,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1107,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1130,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1219,8 @@
         <v>9</v>
       </c>
       <c r="G19">
-        <v>360</v>
+        <f>970-730</f>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1156,9 +1242,9 @@
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="G20">
-        <f>1000-720</f>
-        <v>280</v>
+      <c r="G20" s="9">
+        <f>1650-690</f>
+        <v>960</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1181,7 +1267,7 @@
         <v>9</v>
       </c>
       <c r="G21">
-        <f>570-250</f>
+        <f>730-410</f>
         <v>320</v>
       </c>
     </row>
@@ -1204,9 +1290,9 @@
       <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G22">
-        <f>490-170</f>
-        <v>320</v>
+      <c r="G22" s="9">
+        <f>1370-170</f>
+        <v>1200</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1305,26 +1391,26 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="19">
         <v>50</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="19">
         <v>200</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="19">
         <v>5</v>
       </c>
     </row>
@@ -1356,10 +1442,13 @@
       <c r="F34" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="9">
         <f>1560-0</f>
         <v>1560</v>
       </c>
+      <c r="H34" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1380,7 +1469,7 @@
       <c r="F35" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="9">
         <f>2080-440</f>
         <v>1640</v>
       </c>
@@ -1405,8 +1494,7 @@
         <v>9</v>
       </c>
       <c r="G36">
-        <f>730-410</f>
-        <v>320</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1428,9 +1516,9 @@
       <c r="F37" t="s">
         <v>8</v>
       </c>
-      <c r="G37">
-        <f>730-410</f>
-        <v>320</v>
+      <c r="G37" s="9">
+        <f>1980-460</f>
+        <v>1520</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1444,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>0.51200000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="E38">
         <v>25</v>
@@ -1453,8 +1541,8 @@
         <v>9</v>
       </c>
       <c r="G38">
-        <f>810-450</f>
-        <v>360</v>
+        <f>420-180</f>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1468,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>0.51200000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="E39">
         <v>25</v>
@@ -1476,209 +1564,416 @@
       <c r="F39" t="s">
         <v>8</v>
       </c>
-      <c r="G39">
-        <f>530-250</f>
+      <c r="G39" s="9">
+        <f>1980-780</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.75</v>
+      </c>
+      <c r="E40">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="9">
+        <f>1140-20</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="E41">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41">
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="E42">
+        <v>25</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42">
+        <f>480</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B47" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12" t="s">
+      <c r="C47" s="21"/>
+      <c r="D47" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="7" t="s">
+      <c r="E47" s="22"/>
+      <c r="F47" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12" t="s">
+      <c r="G47" s="21"/>
+      <c r="H47" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I44" s="8"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+      <c r="I47" s="22"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B48" s="7">
         <v>16234</v>
       </c>
-      <c r="C45" s="13">
-        <f>B45/SUM(B$45:B$49)</f>
+      <c r="C48" s="10">
+        <f>B48/SUM(B$48:B$52)</f>
         <v>0.66432049760608913</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D48" s="11">
         <v>16251</v>
       </c>
-      <c r="E45" s="15">
-        <f>D45/SUM(D$45:D$49)</f>
+      <c r="E48" s="12">
+        <f>D48/SUM(D$48:D$52)</f>
         <v>0.66501616401358599</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F48" s="7">
         <v>12885</v>
       </c>
-      <c r="G45" s="13">
-        <f>F45/SUM(F$45:F$49)</f>
+      <c r="G48" s="10">
+        <f>F48/SUM(F$48:F$52)</f>
         <v>0.81736868815021568</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H48" s="11">
         <v>14687</v>
       </c>
-      <c r="I45" s="15">
-        <f>H45/SUM(H$45:H$49)</f>
+      <c r="I48" s="12">
+        <f>H48/SUM(H$48:H$52)</f>
         <v>0.93167977670641966</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B49" s="7">
         <v>4946</v>
       </c>
-      <c r="C46" s="13">
-        <f t="shared" ref="C46:C49" si="0">B46/SUM(B$45:B$49)</f>
+      <c r="C49" s="10">
+        <f t="shared" ref="C49:C52" si="0">B49/SUM(B$48:B$52)</f>
         <v>0.20239800302819494</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D49" s="11">
         <v>0</v>
       </c>
-      <c r="E46" s="15">
-        <f>D46/SUM(D$45:D$49)</f>
+      <c r="E49" s="12">
+        <f>D49/SUM(D$48:D$52)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F49" s="7">
         <v>2098</v>
       </c>
-      <c r="G46" s="13">
-        <f t="shared" ref="G46:G49" si="1">F46/SUM(F$45:F$49)</f>
+      <c r="G49" s="10">
+        <f t="shared" ref="G49:G52" si="1">F49/SUM(F$48:F$52)</f>
         <v>0.13308804871859933</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H49" s="11">
         <v>0</v>
       </c>
-      <c r="I46" s="15">
-        <f>H46/SUM(H$45:H$49)</f>
+      <c r="I49" s="12">
+        <f>H49/SUM(H$48:H$52)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B50" s="7">
         <v>582</v>
       </c>
-      <c r="C47" s="13">
+      <c r="C50" s="10">
         <f t="shared" si="0"/>
         <v>2.3816344068420838E-2</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D50" s="11">
         <v>582</v>
       </c>
-      <c r="E47" s="15">
-        <f>D47/SUM(D$45:D$49)</f>
+      <c r="E50" s="12">
+        <f>D50/SUM(D$48:D$52)</f>
         <v>2.3816344068420838E-2</v>
       </c>
-      <c r="F47" s="9">
+      <c r="F50" s="7">
         <v>288</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G50" s="10">
         <f t="shared" si="1"/>
         <v>1.8269474752600864E-2</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H50" s="11">
         <v>288</v>
       </c>
-      <c r="I47" s="15">
-        <f>H47/SUM(H$45:H$49)</f>
+      <c r="I50" s="12">
+        <f>H50/SUM(H$48:H$52)</f>
         <v>1.8269474752600864E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B51" s="7">
         <v>582</v>
       </c>
-      <c r="C48" s="13">
+      <c r="C51" s="10">
         <f t="shared" si="0"/>
         <v>2.3816344068420838E-2</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D51" s="11">
         <v>582</v>
       </c>
-      <c r="E48" s="15">
-        <f>D48/SUM(D$45:D$49)</f>
+      <c r="E51" s="12">
+        <f>D51/SUM(D$48:D$52)</f>
         <v>2.3816344068420838E-2</v>
       </c>
-      <c r="F48" s="9">
+      <c r="F51" s="7">
         <v>288</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G51" s="10">
         <f t="shared" si="1"/>
         <v>1.8269474752600864E-2</v>
       </c>
-      <c r="H48" s="14">
+      <c r="H51" s="11">
         <v>288</v>
       </c>
-      <c r="I48" s="15">
-        <f>H48/SUM(H$45:H$49)</f>
+      <c r="I51" s="12">
+        <f>H51/SUM(H$48:H$52)</f>
         <v>1.8269474752600864E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B52" s="8">
         <v>2093</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C52" s="13">
         <f t="shared" si="0"/>
         <v>8.5648811228874244E-2</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D52" s="14">
         <v>7022</v>
       </c>
-      <c r="E49" s="18">
-        <f>D49/SUM(D$45:D$49)</f>
+      <c r="E52" s="15">
+        <f>D52/SUM(D$48:D$52)</f>
         <v>0.28735114784957239</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F52" s="8">
         <v>205</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G52" s="13">
         <f t="shared" si="1"/>
         <v>1.3004313625983253E-2</v>
       </c>
-      <c r="H49" s="17">
+      <c r="H52" s="14">
         <v>501</v>
       </c>
-      <c r="I49" s="18">
-        <f>H49/SUM(H$45:H$49)</f>
+      <c r="I52" s="15">
+        <f>H52/SUM(H$48:H$52)</f>
         <v>3.1781273788378583E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="6"/>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="22"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="22"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="7">
+        <v>15790</v>
+      </c>
+      <c r="C55" s="10">
+        <f>B55/SUM(B$55:B$59)</f>
+        <v>0.83083399105498557</v>
+      </c>
+      <c r="D55" s="11">
+        <v>17629</v>
+      </c>
+      <c r="E55" s="10">
+        <f t="shared" ref="E55:E59" si="2">D55/SUM(D$55:D$59)</f>
+        <v>0.92657416167349937</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="7">
+        <v>2217</v>
+      </c>
+      <c r="C56" s="10">
+        <f t="shared" ref="C56:C59" si="3">B56/SUM(B$55:B$59)</f>
+        <v>0.11665351223362273</v>
+      </c>
+      <c r="D56" s="11">
+        <v>0</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="7">
+        <v>289</v>
+      </c>
+      <c r="C57" s="10">
+        <f t="shared" si="3"/>
+        <v>1.5206524598789793E-2</v>
+      </c>
+      <c r="D57" s="11">
+        <v>289</v>
+      </c>
+      <c r="E57" s="10">
+        <f t="shared" si="2"/>
+        <v>1.518974035530327E-2</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="7">
+        <v>289</v>
+      </c>
+      <c r="C58" s="10">
+        <f t="shared" si="3"/>
+        <v>1.5206524598789793E-2</v>
+      </c>
+      <c r="D58" s="11">
+        <v>289</v>
+      </c>
+      <c r="E58" s="10">
+        <f t="shared" si="2"/>
+        <v>1.518974035530327E-2</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="8">
+        <v>420</v>
+      </c>
+      <c r="C59" s="10">
+        <f t="shared" si="3"/>
+        <v>2.2099447513812154E-2</v>
+      </c>
+      <c r="D59" s="14">
+        <v>819</v>
+      </c>
+      <c r="E59" s="10">
+        <f t="shared" si="2"/>
+        <v>4.3046357615894038E-2</v>
+      </c>
+      <c r="F59" s="8"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="10"/>
     </row>
   </sheetData>
   <sortState ref="A2:G7">
     <sortCondition ref="D2:D7"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
+  <mergeCells count="8">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>